<commit_message>
Ajuste del modelo de usuario al diagrama de clase
</commit_message>
<xml_diff>
--- a/Documentacion/Planificacion Diaria.xlsx
+++ b/Documentacion/Planificacion Diaria.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t>v1.1 Modulo de Medicos</t>
   </si>
@@ -329,72 +329,72 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -700,7 +700,7 @@
   <dimension ref="A2:AO140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18:I18"/>
+      <selection activeCell="B14" sqref="B14:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,285 +710,281 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>40942</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="41" t="s">
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>40943</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="41" t="s">
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>40944</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="41" t="s">
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>40945</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>40946</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>40947</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>40948</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="41" t="s">
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>40949</v>
       </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>40950</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>40951</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="24" t="s">
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>40952</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="29" t="s">
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="35" t="s">
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="37"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="24"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>40953</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="29" t="s">
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="29" t="s">
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="35" t="s">
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="37"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="24"/>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>40954</v>
       </c>
-      <c r="B17" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="29" t="s">
+      <c r="B17" s="39"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="29" t="s">
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="29" t="s">
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="O17" s="30"/>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="35" t="s">
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="S17" s="36"/>
-      <c r="T17" s="36"/>
-      <c r="U17" s="37"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="24"/>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>40955</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="29" t="s">
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="29" t="s">
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="29" t="s">
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="S18" s="30"/>
-      <c r="T18" s="30"/>
-      <c r="U18" s="26"/>
-      <c r="V18" s="24" t="s">
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="21"/>
+      <c r="V18" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="W18" s="24"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="24"/>
+      <c r="W18" s="27"/>
+      <c r="X18" s="27"/>
+      <c r="Y18" s="27"/>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
@@ -1002,36 +998,34 @@
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
-      <c r="J19" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="29" t="s">
+      <c r="J19" s="19"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="O19" s="30"/>
-      <c r="P19" s="30"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="29" t="s">
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="S19" s="30"/>
-      <c r="T19" s="30"/>
-      <c r="U19" s="26"/>
-      <c r="V19" s="33" t="s">
+      <c r="S19" s="20"/>
+      <c r="T19" s="20"/>
+      <c r="U19" s="21"/>
+      <c r="V19" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="W19" s="34"/>
-      <c r="X19" s="34"/>
-      <c r="Y19" s="19"/>
-      <c r="Z19" s="24" t="s">
+      <c r="W19" s="35"/>
+      <c r="X19" s="35"/>
+      <c r="Y19" s="31"/>
+      <c r="Z19" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="AA19" s="24"/>
-      <c r="AB19" s="24"/>
-      <c r="AC19" s="24"/>
+      <c r="AA19" s="27"/>
+      <c r="AB19" s="27"/>
+      <c r="AC19" s="27"/>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
@@ -1045,36 +1039,34 @@
       <c r="K20" s="17"/>
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
-      <c r="N20" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="29" t="s">
+      <c r="N20" s="19"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="S20" s="30"/>
-      <c r="T20" s="30"/>
-      <c r="U20" s="26"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="20"/>
+      <c r="U20" s="21"/>
       <c r="V20" s="6" t="s">
         <v>24</v>
       </c>
       <c r="W20" s="6"/>
       <c r="X20" s="6"/>
       <c r="Y20" s="6"/>
-      <c r="Z20" s="29" t="s">
+      <c r="Z20" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AA20" s="30"/>
-      <c r="AB20" s="30"/>
-      <c r="AC20" s="26"/>
-      <c r="AD20" s="35" t="s">
+      <c r="AA20" s="20"/>
+      <c r="AB20" s="20"/>
+      <c r="AC20" s="21"/>
+      <c r="AD20" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AE20" s="36"/>
-      <c r="AF20" s="36"/>
-      <c r="AG20" s="37"/>
+      <c r="AE20" s="23"/>
+      <c r="AF20" s="23"/>
+      <c r="AG20" s="24"/>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
@@ -1089,36 +1081,34 @@
       <c r="O21" s="17"/>
       <c r="P21" s="17"/>
       <c r="Q21" s="17"/>
-      <c r="R21" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="S21" s="30"/>
-      <c r="T21" s="30"/>
-      <c r="U21" s="26"/>
-      <c r="V21" s="33" t="s">
+      <c r="R21" s="19"/>
+      <c r="S21" s="20"/>
+      <c r="T21" s="20"/>
+      <c r="U21" s="21"/>
+      <c r="V21" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="W21" s="34"/>
-      <c r="X21" s="34"/>
-      <c r="Y21" s="19"/>
-      <c r="Z21" s="29" t="s">
+      <c r="W21" s="35"/>
+      <c r="X21" s="35"/>
+      <c r="Y21" s="31"/>
+      <c r="Z21" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="AA21" s="30"/>
-      <c r="AB21" s="30"/>
-      <c r="AC21" s="26"/>
-      <c r="AD21" s="29" t="s">
+      <c r="AA21" s="20"/>
+      <c r="AB21" s="20"/>
+      <c r="AC21" s="21"/>
+      <c r="AD21" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AE21" s="30"/>
-      <c r="AF21" s="30"/>
-      <c r="AG21" s="26"/>
-      <c r="AH21" s="35" t="s">
+      <c r="AE21" s="20"/>
+      <c r="AF21" s="20"/>
+      <c r="AG21" s="21"/>
+      <c r="AH21" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="AI21" s="36"/>
-      <c r="AJ21" s="36"/>
-      <c r="AK21" s="37"/>
+      <c r="AI21" s="23"/>
+      <c r="AJ21" s="23"/>
+      <c r="AK21" s="24"/>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
@@ -1132,36 +1122,34 @@
       <c r="S22" s="17"/>
       <c r="T22" s="17"/>
       <c r="U22" s="17"/>
-      <c r="V22" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="V22" s="6"/>
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
       <c r="Y22" s="6"/>
-      <c r="Z22" s="29" t="s">
+      <c r="Z22" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="AA22" s="30"/>
-      <c r="AB22" s="30"/>
-      <c r="AC22" s="26"/>
-      <c r="AD22" s="29" t="s">
+      <c r="AA22" s="20"/>
+      <c r="AB22" s="20"/>
+      <c r="AC22" s="21"/>
+      <c r="AD22" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="AE22" s="30"/>
-      <c r="AF22" s="30"/>
-      <c r="AG22" s="26"/>
-      <c r="AH22" s="29" t="s">
+      <c r="AE22" s="20"/>
+      <c r="AF22" s="20"/>
+      <c r="AG22" s="21"/>
+      <c r="AH22" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AI22" s="30"/>
-      <c r="AJ22" s="30"/>
-      <c r="AK22" s="26"/>
-      <c r="AL22" s="24" t="s">
+      <c r="AI22" s="20"/>
+      <c r="AJ22" s="20"/>
+      <c r="AK22" s="21"/>
+      <c r="AL22" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AM22" s="24"/>
-      <c r="AN22" s="24"/>
-      <c r="AO22" s="24"/>
+      <c r="AM22" s="27"/>
+      <c r="AN22" s="27"/>
+      <c r="AO22" s="27"/>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
@@ -1175,30 +1163,30 @@
       <c r="W23" s="17"/>
       <c r="X23" s="17"/>
       <c r="Y23" s="17"/>
-      <c r="Z23" s="29" t="s">
+      <c r="Z23" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="AA23" s="30"/>
-      <c r="AB23" s="30"/>
-      <c r="AC23" s="26"/>
-      <c r="AD23" s="29" t="s">
+      <c r="AA23" s="20"/>
+      <c r="AB23" s="20"/>
+      <c r="AC23" s="21"/>
+      <c r="AD23" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="AE23" s="30"/>
-      <c r="AF23" s="30"/>
-      <c r="AG23" s="26"/>
-      <c r="AH23" s="29" t="s">
+      <c r="AE23" s="20"/>
+      <c r="AF23" s="20"/>
+      <c r="AG23" s="21"/>
+      <c r="AH23" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="AI23" s="30"/>
-      <c r="AJ23" s="30"/>
-      <c r="AK23" s="26"/>
-      <c r="AL23" s="29" t="s">
+      <c r="AI23" s="20"/>
+      <c r="AJ23" s="20"/>
+      <c r="AK23" s="21"/>
+      <c r="AL23" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AM23" s="30"/>
-      <c r="AN23" s="30"/>
-      <c r="AO23" s="26"/>
+      <c r="AM23" s="20"/>
+      <c r="AN23" s="20"/>
+      <c r="AO23" s="21"/>
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
@@ -1212,24 +1200,24 @@
       <c r="AA24" s="17"/>
       <c r="AB24" s="17"/>
       <c r="AC24" s="17"/>
-      <c r="AD24" s="29" t="s">
+      <c r="AD24" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="AE24" s="30"/>
-      <c r="AF24" s="30"/>
-      <c r="AG24" s="26"/>
-      <c r="AH24" s="29" t="s">
+      <c r="AE24" s="20"/>
+      <c r="AF24" s="20"/>
+      <c r="AG24" s="21"/>
+      <c r="AH24" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="AI24" s="30"/>
-      <c r="AJ24" s="30"/>
-      <c r="AK24" s="26"/>
-      <c r="AL24" s="29" t="s">
+      <c r="AI24" s="20"/>
+      <c r="AJ24" s="20"/>
+      <c r="AK24" s="21"/>
+      <c r="AL24" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="AM24" s="30"/>
-      <c r="AN24" s="30"/>
-      <c r="AO24" s="26"/>
+      <c r="AM24" s="20"/>
+      <c r="AN24" s="20"/>
+      <c r="AO24" s="21"/>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
@@ -1244,18 +1232,18 @@
       <c r="AE25" s="17"/>
       <c r="AF25" s="17"/>
       <c r="AG25" s="17"/>
-      <c r="AH25" s="29" t="s">
+      <c r="AH25" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="AI25" s="30"/>
-      <c r="AJ25" s="30"/>
-      <c r="AK25" s="26"/>
-      <c r="AL25" s="29" t="s">
+      <c r="AI25" s="20"/>
+      <c r="AJ25" s="20"/>
+      <c r="AK25" s="21"/>
+      <c r="AL25" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="AM25" s="30"/>
-      <c r="AN25" s="30"/>
-      <c r="AO25" s="26"/>
+      <c r="AM25" s="20"/>
+      <c r="AN25" s="20"/>
+      <c r="AO25" s="21"/>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
@@ -1269,382 +1257,382 @@
       <c r="AI26" s="17"/>
       <c r="AJ26" s="17"/>
       <c r="AK26" s="17"/>
-      <c r="AL26" s="29" t="s">
+      <c r="AL26" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="AM26" s="30"/>
-      <c r="AN26" s="30"/>
-      <c r="AO26" s="26"/>
+      <c r="AM26" s="20"/>
+      <c r="AN26" s="20"/>
+      <c r="AO26" s="21"/>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>40964</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
     </row>
     <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>40965</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20" t="s">
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20" t="s">
+      <c r="G28" s="32"/>
+      <c r="H28" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20" t="s">
+      <c r="I28" s="32"/>
+      <c r="J28" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="K28" s="20"/>
+      <c r="K28" s="32"/>
     </row>
     <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <v>40966</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
         <v>40967</v>
       </c>
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <v>40968</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
       <c r="F31" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="3"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
     </row>
     <row r="32" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
         <v>40969</v>
       </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="16">
         <v>40970</v>
       </c>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <v>40971</v>
       </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
       <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>40972</v>
       </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>40973</v>
       </c>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>40974</v>
       </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="36"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>40975</v>
       </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>40976</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>40977</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40978</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="36"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>40979</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>40980</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>40981</v>
       </c>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>40982</v>
       </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>40983</v>
       </c>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>40984</v>
       </c>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>40985</v>
       </c>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="36"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>40986</v>
       </c>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="36"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>40987</v>
       </c>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="36"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>40988</v>
       </c>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="36"/>
+      <c r="E51" s="36"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>40989</v>
       </c>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="36"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>40990</v>
       </c>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="36"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>40991</v>
       </c>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="36"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>40992</v>
       </c>
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>40993</v>
       </c>
-      <c r="B56" s="25"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="36"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>40994</v>
       </c>
-      <c r="B57" s="25"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="36"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>40995</v>
       </c>
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="36"/>
+      <c r="E58" s="36"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>40996</v>
       </c>
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="25"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="36"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>40997</v>
       </c>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="36"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>40998</v>
       </c>
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="36"/>
+      <c r="D61" s="36"/>
+      <c r="E61" s="36"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="36"/>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
@@ -1843,29 +1831,65 @@
     </row>
   </sheetData>
   <mergeCells count="99">
-    <mergeCell ref="AD22:AG22"/>
-    <mergeCell ref="AD21:AG21"/>
-    <mergeCell ref="AD20:AG20"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H9"/>
-    <mergeCell ref="F11:H12"/>
-    <mergeCell ref="AH25:AK25"/>
-    <mergeCell ref="AH24:AK24"/>
-    <mergeCell ref="AH23:AK23"/>
-    <mergeCell ref="AH22:AK22"/>
-    <mergeCell ref="AH21:AK21"/>
-    <mergeCell ref="N16:Q16"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="N19:Q19"/>
-    <mergeCell ref="N20:Q20"/>
-    <mergeCell ref="AD24:AG24"/>
-    <mergeCell ref="AD23:AG23"/>
-    <mergeCell ref="AL26:AO26"/>
-    <mergeCell ref="AL25:AO25"/>
-    <mergeCell ref="AL24:AO24"/>
-    <mergeCell ref="AL23:AO23"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="Z19:AC19"/>
+    <mergeCell ref="Z20:AC20"/>
+    <mergeCell ref="Z21:AC21"/>
+    <mergeCell ref="Z22:AC22"/>
+    <mergeCell ref="Z23:AC23"/>
+    <mergeCell ref="V18:Y18"/>
+    <mergeCell ref="V19:Y19"/>
+    <mergeCell ref="V21:Y21"/>
+    <mergeCell ref="R17:U17"/>
+    <mergeCell ref="R18:U18"/>
+    <mergeCell ref="R19:U19"/>
+    <mergeCell ref="R20:U20"/>
+    <mergeCell ref="R21:U21"/>
+    <mergeCell ref="B5:E6"/>
     <mergeCell ref="AL22:AO22"/>
     <mergeCell ref="B7:E9"/>
     <mergeCell ref="B10:E10"/>
@@ -1882,66 +1906,30 @@
     <mergeCell ref="J28:K28"/>
     <mergeCell ref="B27:K27"/>
     <mergeCell ref="B13:E13"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="Z19:AC19"/>
-    <mergeCell ref="Z20:AC20"/>
-    <mergeCell ref="Z21:AC21"/>
-    <mergeCell ref="Z22:AC22"/>
-    <mergeCell ref="Z23:AC23"/>
-    <mergeCell ref="V18:Y18"/>
-    <mergeCell ref="V19:Y19"/>
-    <mergeCell ref="V21:Y21"/>
-    <mergeCell ref="R17:U17"/>
-    <mergeCell ref="R18:U18"/>
-    <mergeCell ref="R19:U19"/>
-    <mergeCell ref="R20:U20"/>
-    <mergeCell ref="R21:U21"/>
-    <mergeCell ref="B5:E6"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="AD24:AG24"/>
+    <mergeCell ref="AD23:AG23"/>
+    <mergeCell ref="AL26:AO26"/>
+    <mergeCell ref="AL25:AO25"/>
+    <mergeCell ref="AL24:AO24"/>
+    <mergeCell ref="AL23:AO23"/>
+    <mergeCell ref="AH25:AK25"/>
+    <mergeCell ref="AH24:AK24"/>
+    <mergeCell ref="AH23:AK23"/>
+    <mergeCell ref="AH22:AK22"/>
+    <mergeCell ref="AH21:AK21"/>
+    <mergeCell ref="AD22:AG22"/>
+    <mergeCell ref="AD21:AG21"/>
+    <mergeCell ref="AD20:AG20"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H9"/>
+    <mergeCell ref="F11:H12"/>
+    <mergeCell ref="N16:Q16"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="N20:Q20"/>
     <mergeCell ref="F14:I14"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>